<commit_message>
products multi select, download, delete, add, and update
</commit_message>
<xml_diff>
--- a/public/assets/product-import-template.xlsx
+++ b/public/assets/product-import-template.xlsx
@@ -67,19 +67,19 @@
     <t xml:space="preserve">demo</t>
   </si>
   <si>
-    <t xml:space="preserve">c3854ea7-4fdf-49f0-aa31-847acf28ad5a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0ebfad6c-d81f-48c3-9b2b-02ec8e6cdad3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6f7e6a00-7c8b-45ba-8336-145254d71548</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca5ea1da-df1c-4e5e-baba-3be5c63daa1f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8f6e8bac-de2d-4d29-b108-0525fc66d8e0</t>
+    <t xml:space="preserve">f243adf4-1cf7-40e7-941c-9549dc987b95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f6e4a2b9-bdd7-44de-97b9-b5f6f2588a20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbf7c588-eb3f-4a12-9f03-0c71d4365c25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">959db27b-15be-471c-acaa-e0ea81168803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7e6d3758-aad6-4e5c-948b-9d15303d0e1c</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -111,12 +111,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +160,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,7 +184,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
update product upload template
</commit_message>
<xml_diff>
--- a/public/assets/product-import-template.xlsx
+++ b/public/assets/product-import-template.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
   <si>
     <t xml:space="preserve">productID</t>
   </si>
@@ -181,29 +184,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.32"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -240,34 +243,34 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>17</v>
@@ -278,26 +281,29 @@
       <c r="L2" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="M2" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Properly calculate tax and discount in quotation
</commit_message>
<xml_diff>
--- a/public/assets/product-import-template.xlsx
+++ b/public/assets/product-import-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">taxRateId</t>
-  </si>
-  <si>
     <t xml:space="preserve">quantity</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
   </si>
   <si>
     <t xml:space="preserve">demo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f243adf4-1cf7-40e7-941c-9549dc987b95</t>
   </si>
   <si>
     <t xml:space="preserve">f6e4a2b9-bdd7-44de-97b9-b5f6f2588a20</t>
@@ -187,10 +181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -198,16 +192,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,70 +244,59 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="K2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>4000</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-      <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-      <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
-      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>